<commit_message>
day-25 capstone project update
</commit_message>
<xml_diff>
--- a/2025-06-06/Documentation.xlsx
+++ b/2025-06-06/Documentation.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hayagreevanv/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC55563-2215-ED45-841C-9C758921C943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9D3422-36AF-C94F-87E2-8676589F00E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="660" windowWidth="35520" windowHeight="20200" xr2:uid="{76326FFE-E4D5-6748-9076-53B704CE8977}"/>
+    <workbookView xWindow="160" yWindow="660" windowWidth="35520" windowHeight="20200" activeTab="1" xr2:uid="{76326FFE-E4D5-6748-9076-53B704CE8977}"/>
   </bookViews>
   <sheets>
-    <sheet name="API Routes" sheetId="1" r:id="rId1"/>
-    <sheet name="Database Schema" sheetId="2" r:id="rId2"/>
+    <sheet name="Database Schema" sheetId="2" r:id="rId1"/>
+    <sheet name="API Routes" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="121">
   <si>
     <t>Authentication Controller</t>
   </si>
@@ -394,6 +394,12 @@
   </si>
   <si>
     <t>Refresh_Token Table</t>
+  </si>
+  <si>
+    <t>/api/v1/users/revoke/{id}</t>
+  </si>
+  <si>
+    <t>Revoke Deleted User or Change User's Role</t>
   </si>
 </sst>
 </file>
@@ -494,6 +500,294 @@
   <dxfs count="48">
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -940,294 +1234,6 @@
         <name val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
       </font>
     </dxf>
   </dxfs>
@@ -1244,104 +1250,104 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4D54619E-1847-5D45-8643-49E7C96DF794}" name="Table1" displayName="Table1" ref="A5:D9" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
-  <autoFilter ref="A5:D9" xr:uid="{4D54619E-1847-5D45-8643-49E7C96DF794}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{EC3F468E-CAF8-3249-B756-7D9A8C6A9CA3}" name="Table4" displayName="Table4" ref="A4:D14" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+  <autoFilter ref="A4:D14" xr:uid="{EC3F468E-CAF8-3249-B756-7D9A8C6A9CA3}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CF092AA9-3A77-F047-811C-5831C0B2E9EE}" name="Routes" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{C911EF16-645B-4D4F-BC7D-C9BB17935A37}" name="Methods" dataDxfId="44"/>
-    <tableColumn id="3" xr3:uid="{2229B047-13AE-AE49-AE20-29ACD12E8F2D}" name="Authorization" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{CF908B81-467C-9B41-A0EE-05805A1B2A7C}" name="Description" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{94B8C535-7BD9-214D-9D84-6019ED34E2FE}" name="Column Name" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{E88D8EB2-A092-5A49-B699-722C6AF5F1AA}" name="Data Type" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{9E5294FE-4E6A-CD4D-9300-E9CAC035D8B8}" name="Constraints" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{DE3CBABE-7D1C-E04F-8001-CDB9C80CD73B}" name="Description" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6A75D630-F969-F14E-AA3B-F5FD75F03E5F}" name="Table13" displayName="Table13" ref="A16:D22" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
-  <autoFilter ref="A16:D22" xr:uid="{6A75D630-F969-F14E-AA3B-F5FD75F03E5F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A11293CD-620A-1F49-9C59-D90D8BE7D47B}" name="Table5" displayName="Table5" ref="A19:D27" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+  <autoFilter ref="A19:D27" xr:uid="{A11293CD-620A-1F49-9C59-D90D8BE7D47B}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{EA86A47D-8652-4841-91B0-6CCA9A021E6F}" name="Routes" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{3F4FD8CA-B088-D642-97E5-EBCC9C5B6B56}" name="Methods" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{902431BD-B0E5-9549-82CD-0E9920235E4E}" name="Authorization" dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{13850D9C-D75C-5946-8071-B81DFE3DB7F1}" name="Description" dataDxfId="36"/>
+    <tableColumn id="1" xr3:uid="{6720F9DB-D33A-F847-BC6A-4D4FECACA2E3}" name="Column Name" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{88630407-2759-634B-AEE5-C79F8A540AE0}" name="Data Type" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{CF201154-F8EE-A846-BEF1-AD2BF2CE2491}" name="Constraints" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{5CE60891-2904-B041-B147-1F8DAE337B94}" name="Description" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{64DC0AFD-092F-B441-A8F6-B51D261CCC33}" name="Table134" displayName="Table134" ref="A29:D36" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
-  <autoFilter ref="A29:D36" xr:uid="{64DC0AFD-092F-B441-A8F6-B51D261CCC33}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{DBF93727-B50F-5646-8F1E-14D9FA27DC5D}" name="Table6" displayName="Table6" ref="A32:D39" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+  <autoFilter ref="A32:D39" xr:uid="{DBF93727-B50F-5646-8F1E-14D9FA27DC5D}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{0247796F-2A0B-5C48-8065-4619DF4F1F86}" name="Routes" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{9FCB6066-EDB5-1444-8726-F94D4E4A44C7}" name="Methods" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{86A28E62-5FAA-B149-BB1E-0544FA8D14DE}" name="Authorization" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{A8B5C909-32A1-8D4D-B8DB-C5F14B600C96}" name="Description" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{44DD5F70-C56C-E940-A5EE-9524ED229A41}" name="Column Name" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{2A09ED4E-5DD7-2948-99D2-8268DBD2A1B8}" name="Data Type" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{6EE86719-EFD4-A045-89F4-56CD0FB27A42}" name="Constraints" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{F6CC6334-2C54-914C-9F47-8B11C755CA24}" name="Description" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{EC3F468E-CAF8-3249-B756-7D9A8C6A9CA3}" name="Table4" displayName="Table4" ref="A4:D14" totalsRowShown="0" headerRowDxfId="24" dataDxfId="25">
-  <autoFilter ref="A4:D14" xr:uid="{EC3F468E-CAF8-3249-B756-7D9A8C6A9CA3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B2AC4FB5-20D2-5A46-BD20-E88BAE106AF7}" name="Table7" displayName="Table7" ref="A44:D51" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+  <autoFilter ref="A44:D51" xr:uid="{B2AC4FB5-20D2-5A46-BD20-E88BAE106AF7}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{94B8C535-7BD9-214D-9D84-6019ED34E2FE}" name="Column Name" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{E88D8EB2-A092-5A49-B699-722C6AF5F1AA}" name="Data Type" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{9E5294FE-4E6A-CD4D-9300-E9CAC035D8B8}" name="Constraints" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{DE3CBABE-7D1C-E04F-8001-CDB9C80CD73B}" name="Description" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{04AE0F79-CA38-944F-BE49-3F9709F59C31}" name="Column Name" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{EE65FDA2-DC36-0A4D-8B17-E1DA8CD29AD7}" name="Data Type" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{B7935034-29EC-0543-BE88-2AE0E45BB343}" name="Constraints" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{BC2313E7-BC07-AE4B-BA90-89FDDDF7927F}" name="Description" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A11293CD-620A-1F49-9C59-D90D8BE7D47B}" name="Table5" displayName="Table5" ref="A19:D27" totalsRowShown="0" headerRowDxfId="18" dataDxfId="19">
-  <autoFilter ref="A19:D27" xr:uid="{A11293CD-620A-1F49-9C59-D90D8BE7D47B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{18CD9C58-83EC-9144-84B7-7A2F8CBCFE05}" name="Table8" displayName="Table8" ref="A56:D58" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="A56:D58" xr:uid="{18CD9C58-83EC-9144-84B7-7A2F8CBCFE05}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6720F9DB-D33A-F847-BC6A-4D4FECACA2E3}" name="Column Name" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{88630407-2759-634B-AEE5-C79F8A540AE0}" name="Data Type" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{CF201154-F8EE-A846-BEF1-AD2BF2CE2491}" name="Constraints" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{5CE60891-2904-B041-B147-1F8DAE337B94}" name="Description" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{33DB6D78-C8CF-E842-AC49-56213DB2EB41}" name="Column Name" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{B8DF1B90-68D5-B04E-A872-DFE1A5DC8A9E}" name="Data Type" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{9320429C-5507-FB46-BBBD-5FE3E7D27308}" name="Constraints" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{A923D3A7-B830-CC4A-9834-4C34A0560FD7}" name="Description" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{DBF93727-B50F-5646-8F1E-14D9FA27DC5D}" name="Table6" displayName="Table6" ref="A32:D39" totalsRowShown="0" headerRowDxfId="12" dataDxfId="13">
-  <autoFilter ref="A32:D39" xr:uid="{DBF93727-B50F-5646-8F1E-14D9FA27DC5D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4D54619E-1847-5D45-8643-49E7C96DF794}" name="Table1" displayName="Table1" ref="A5:D9" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A5:D9" xr:uid="{4D54619E-1847-5D45-8643-49E7C96DF794}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{44DD5F70-C56C-E940-A5EE-9524ED229A41}" name="Column Name" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{2A09ED4E-5DD7-2948-99D2-8268DBD2A1B8}" name="Data Type" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{6EE86719-EFD4-A045-89F4-56CD0FB27A42}" name="Constraints" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{F6CC6334-2C54-914C-9F47-8B11C755CA24}" name="Description" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{CF092AA9-3A77-F047-811C-5831C0B2E9EE}" name="Routes" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{C911EF16-645B-4D4F-BC7D-C9BB17935A37}" name="Methods" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{2229B047-13AE-AE49-AE20-29ACD12E8F2D}" name="Authorization" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{CF908B81-467C-9B41-A0EE-05805A1B2A7C}" name="Description" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B2AC4FB5-20D2-5A46-BD20-E88BAE106AF7}" name="Table7" displayName="Table7" ref="A44:D51" totalsRowShown="0" headerRowDxfId="6" dataDxfId="7">
-  <autoFilter ref="A44:D51" xr:uid="{B2AC4FB5-20D2-5A46-BD20-E88BAE106AF7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6A75D630-F969-F14E-AA3B-F5FD75F03E5F}" name="Table13" displayName="Table13" ref="A16:D22" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A16:D22" xr:uid="{6A75D630-F969-F14E-AA3B-F5FD75F03E5F}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{04AE0F79-CA38-944F-BE49-3F9709F59C31}" name="Column Name" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{EE65FDA2-DC36-0A4D-8B17-E1DA8CD29AD7}" name="Data Type" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{B7935034-29EC-0543-BE88-2AE0E45BB343}" name="Constraints" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{BC2313E7-BC07-AE4B-BA90-89FDDDF7927F}" name="Description" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{EA86A47D-8652-4841-91B0-6CCA9A021E6F}" name="Routes" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{3F4FD8CA-B088-D642-97E5-EBCC9C5B6B56}" name="Methods" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{902431BD-B0E5-9549-82CD-0E9920235E4E}" name="Authorization" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{13850D9C-D75C-5946-8071-B81DFE3DB7F1}" name="Description" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{18CD9C58-83EC-9144-84B7-7A2F8CBCFE05}" name="Table8" displayName="Table8" ref="A56:D58" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A56:D58" xr:uid="{18CD9C58-83EC-9144-84B7-7A2F8CBCFE05}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{64DC0AFD-092F-B441-A8F6-B51D261CCC33}" name="Table134" displayName="Table134" ref="A29:D37" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A29:D37" xr:uid="{64DC0AFD-092F-B441-A8F6-B51D261CCC33}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{33DB6D78-C8CF-E842-AC49-56213DB2EB41}" name="Column Name" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{B8DF1B90-68D5-B04E-A872-DFE1A5DC8A9E}" name="Data Type" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{9320429C-5507-FB46-BBBD-5FE3E7D27308}" name="Constraints" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{A923D3A7-B830-CC4A-9834-4C34A0560FD7}" name="Description" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{0247796F-2A0B-5C48-8065-4619DF4F1F86}" name="Routes" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{9FCB6066-EDB5-1444-8726-F94D4E4A44C7}" name="Methods" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{86A28E62-5FAA-B149-BB1E-0544FA8D14DE}" name="Authorization" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{A8B5C909-32A1-8D4D-B8DB-C5F14B600C96}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1663,452 +1669,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FBD7142-294A-7243-9D07-FDB56C1026ED}">
-  <dimension ref="A1:E43"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="40" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" customWidth="1"/>
-    <col min="4" max="4" width="45.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="22" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" ht="22" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" ht="22" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" ht="22" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" ht="22" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" ht="22" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" ht="22" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" ht="22" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" ht="22" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" ht="22" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" ht="22" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" ht="22" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" ht="22" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" ht="22" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" ht="22" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" ht="22" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="22" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="22" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="22" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="22" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="22" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="92" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="22" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="26" spans="1:4" ht="22" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="1:4" ht="22" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="1:4" ht="22" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="1:4" ht="22" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="22" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="22" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="22" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="22" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="22" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="22" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="23" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="22" x14ac:dyDescent="0.3">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-    </row>
-    <row r="39" spans="1:4" ht="22" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B39" s="1"/>
-    </row>
-    <row r="40" spans="1:4" ht="22" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B40" s="1"/>
-    </row>
-    <row r="41" spans="1:4" ht="22" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B41" s="1"/>
-    </row>
-    <row r="42" spans="1:4" ht="22" x14ac:dyDescent="0.3">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-    </row>
-    <row r="43" spans="1:4" ht="22" x14ac:dyDescent="0.3">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="3">
-    <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A5E15F4-2B92-B840-B516-DFEFFE594C5E}">
   <dimension ref="A2:D58"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" x14ac:dyDescent="0.3"/>
@@ -2723,4 +2288,459 @@
     <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FBD7142-294A-7243-9D07-FDB56C1026ED}">
+  <dimension ref="A1:E44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="40" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="52" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="22" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" ht="22" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" ht="22" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" ht="22" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" ht="22" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" ht="22" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" ht="22" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" ht="22" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" ht="22" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" ht="22" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" ht="22" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" ht="22" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" ht="22" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" ht="22" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" ht="22" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" ht="22" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="22" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="22" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="22" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="22" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="22" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="92" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="22" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="26" spans="1:4" ht="22" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="1:4" ht="22" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="1:4" ht="22" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="1:4" ht="22" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="22" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="22" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="22" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="22" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="22" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="22" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="23" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="23" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="22" x14ac:dyDescent="0.3">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+    </row>
+    <row r="40" spans="1:4" ht="22" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" s="1"/>
+    </row>
+    <row r="41" spans="1:4" ht="22" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41" s="1"/>
+    </row>
+    <row r="42" spans="1:4" ht="22" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" s="1"/>
+    </row>
+    <row r="43" spans="1:4" ht="22" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="1:4" ht="22" x14ac:dyDescent="0.3">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="3">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>